<commit_message>
Model-driven expression parsing rules
</commit_message>
<xml_diff>
--- a/editor-models/generated-models/src/main/resources/SharpOperators.xlsx
+++ b/editor-models/generated-models/src/main/resources/SharpOperators.xlsx
@@ -1518,8 +1518,8 @@
   </sheetPr>
   <dimension ref="A1:AN117"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A56" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="L72" activeCellId="0" pane="topLeft" sqref="L72"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="N35" activeCellId="0" pane="topLeft" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -2309,7 +2309,7 @@
         <v>83</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="28">
@@ -2375,7 +2375,7 @@
       <c r="C29" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G29" s="0" t="s">
+      <c r="G29" s="2" t="s">
         <v>91</v>
       </c>
       <c r="I29" s="2" t="s">
@@ -3244,7 +3244,7 @@
       <c r="C67" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G67" s="0" t="s">
+      <c r="G67" s="2" t="s">
         <v>163</v>
       </c>
       <c r="I67" s="2" t="s">
@@ -3348,7 +3348,7 @@
       <c r="C71" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G71" s="0" t="s">
+      <c r="G71" s="2" t="s">
         <v>163</v>
       </c>
       <c r="I71" s="2" t="s">
@@ -3364,7 +3364,7 @@
         <v>164</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="72">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="72">
       <c r="A72" s="2" t="s">
         <v>174</v>
       </c>
@@ -3978,7 +3978,7 @@
       <c r="C104" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G104" s="0" t="s">
+      <c r="G104" s="2" t="s">
         <v>163</v>
       </c>
       <c r="I104" s="2" t="s">
@@ -4599,8 +4599,7 @@
     <col collapsed="false" hidden="false" max="3" min="1" style="0" width="27.3673469387755"/>
     <col collapsed="false" hidden="false" max="11" min="4" style="0" width="8.72959183673469"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15"/>
-    <col collapsed="false" hidden="false" max="40" min="13" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="41" style="2" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="1" s="2">
@@ -6577,7 +6576,7 @@
   <dimension ref="A1:I149"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100">
-      <pane activePane="bottomLeft" state="split" topLeftCell="A19" xSplit="0" ySplit="6750"/>
+      <pane activePane="bottomLeft" state="split" topLeftCell="A19" xSplit="0" ySplit="6780"/>
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
       <selection activeCell="A35" activeCellId="0" pane="bottomLeft" sqref="A35"/>
     </sheetView>

</xml_diff>

<commit_message>
Fix ontologies and operators, support datatypes, reflective visitor to export expressions
</commit_message>
<xml_diff>
--- a/editor-models/generated-models/src/main/resources/SharpOperators.xlsx
+++ b/editor-models/generated-models/src/main/resources/SharpOperators.xlsx
@@ -255,19 +255,19 @@
     <t>valueType</t>
   </si>
   <si>
+    <t>PhysicalQuantityLiteral</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>UrlLiteral</t>
+  </si>
+  <si>
+    <t>capabilities</t>
+  </si>
+  <si>
     <t>xsd:anyURI</t>
-  </si>
-  <si>
-    <t>PhysicalQuantityLiteral</t>
-  </si>
-  <si>
-    <t>unit</t>
-  </si>
-  <si>
-    <t>UrlLiteral</t>
-  </si>
-  <si>
-    <t>capabilities</t>
   </si>
   <si>
     <t>RealLiteral</t>
@@ -1518,8 +1518,8 @@
   </sheetPr>
   <dimension ref="A1:AN117"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="N35" activeCellId="0" pane="topLeft" sqref="N35"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A36" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="L52" activeCellId="0" pane="topLeft" sqref="L52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -2039,7 +2039,7 @@
         <v>54</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>19</v>
@@ -2050,7 +2050,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="16">
       <c r="A16" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B16" s="2" t="n">
         <v>-99</v>
@@ -2065,7 +2065,7 @@
         <v>28</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>24</v>
@@ -2073,7 +2073,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="17">
       <c r="A17" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B17" s="2" t="n">
         <v>-99</v>
@@ -2082,7 +2082,7 @@
         <v>39</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>24</v>
@@ -2097,7 +2097,7 @@
         <v>19</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="18">
@@ -2871,7 +2871,7 @@
         <v>54</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="57">
@@ -3841,7 +3841,7 @@
         <v>203</v>
       </c>
       <c r="J95" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="96">
@@ -4778,13 +4778,13 @@
         <v>16</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>11</v>
@@ -4862,7 +4862,7 @@
         <v>35</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q7" s="2" t="s">
         <v>36</v>
@@ -5076,7 +5076,7 @@
         <v>54</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>19</v>
@@ -5087,7 +5087,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="16">
       <c r="A16" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B16" s="2" t="n">
         <v>-99</v>
@@ -5099,7 +5099,7 @@
         <v>28</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>24</v>
@@ -5107,13 +5107,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="17">
       <c r="A17" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B17" s="2" t="n">
         <v>-99</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>24</v>
@@ -5128,7 +5128,7 @@
         <v>19</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="18">
@@ -5620,7 +5620,7 @@
         <v>54</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="57">
@@ -5729,7 +5729,7 @@
         <v>144</v>
       </c>
       <c r="X61" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="62">
@@ -5791,7 +5791,7 @@
         <v>144</v>
       </c>
       <c r="AD62" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="AE62" s="2" t="s">
         <v>139</v>
@@ -5980,7 +5980,7 @@
         <v>173</v>
       </c>
       <c r="L71" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="72">
@@ -6290,7 +6290,7 @@
         <v>201</v>
       </c>
       <c r="J94" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="95">
@@ -6304,7 +6304,7 @@
         <v>203</v>
       </c>
       <c r="J95" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="96">
@@ -6372,7 +6372,7 @@
         <v>212</v>
       </c>
       <c r="L102" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="103">
@@ -6400,7 +6400,7 @@
         <v>173</v>
       </c>
       <c r="L104" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="105">
@@ -6576,7 +6576,7 @@
   <dimension ref="A1:I149"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100">
-      <pane activePane="bottomLeft" state="split" topLeftCell="A19" xSplit="0" ySplit="6780"/>
+      <pane activePane="bottomLeft" state="split" topLeftCell="A19" xSplit="0" ySplit="6840"/>
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
       <selection activeCell="A35" activeCellId="0" pane="bottomLeft" sqref="A35"/>
     </sheetView>

</xml_diff>